<commit_message>
Lägger till category och title
och gör om allt till små bokstäver
</commit_message>
<xml_diff>
--- a/traning.xlsx
+++ b/traning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vike_\excelförsök\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vhemm\Documents\GitHub\Examensarbete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63892D1A-5797-4A8F-98FB-57777052CC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B85DB3-198B-4033-9347-CF4518D9208D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10050" yWindow="3735" windowWidth="21600" windowHeight="11505" xr2:uid="{D28E50AB-BE5F-4797-A14B-38F9564C3B92}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D28E50AB-BE5F-4797-A14B-38F9564C3B92}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Konstnar</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>METICOLOUS</t>
+  </si>
+  <si>
+    <t>Idrottare</t>
+  </si>
+  <si>
+    <t>FYSISK</t>
   </si>
 </sst>
 </file>
@@ -422,15 +428,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66667D3-FBB8-4EF6-A017-146B99D11EC4}">
-  <dimension ref="A2:B4"/>
+  <dimension ref="A2:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -438,7 +444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -446,7 +452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -454,12 +460,29 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A1A01BD1BF7C214E96E3D43559DD3656" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fe6fd6ca5621d8c80b73f2da84882b1e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="23d83626-79b6-450d-b59b-ad64057fd917" xmlns:ns4="d51c6c93-62ac-4496-a38c-790379899b3e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c0563089bcae06412ab459a1a6156efa" ns3:_="" ns4:_="">
     <xsd:import namespace="23d83626-79b6-450d-b59b-ad64057fd917"/>
@@ -684,15 +707,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -702,6 +716,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9390050-1D48-41F7-B1E9-92ECABF10612}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C3C6341-759F-438B-BB27-11B8D7B2AC88}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -720,14 +742,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9390050-1D48-41F7-B1E9-92ECABF10612}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1C94AAA-5BEF-49A3-B911-F86248837EFB}">
   <ds:schemaRefs>

</xml_diff>